<commit_message>
Deleted depricated content in excel - nothing serious
</commit_message>
<xml_diff>
--- a/example_template.xlsx
+++ b/example_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\brightway\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9474C664-3F79-486C-A170-85BC38C1D709}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DA0EA9-C2F9-4D37-B83A-BAEAF111DAE4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="138">
   <si>
     <t>skip</t>
   </si>
@@ -163,19 +163,7 @@
     <t>none</t>
   </si>
   <si>
-    <t>Example LCI:</t>
-  </si>
-  <si>
     <t>UFO</t>
-  </si>
-  <si>
-    <t>Image, of how activities and exchanges interact with each other</t>
-  </si>
-  <si>
-    <t>Fuel: Gulp, which is a mix of dirty chai and rainbow drops</t>
-  </si>
-  <si>
-    <t>UFO production scenarios with energy mix, atom, PV/wind</t>
   </si>
   <si>
     <t>UFO production</t>
@@ -1284,18 +1272,18 @@
         <v>0</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="18"/>
       <c r="B2" s="18" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1339,7 +1327,7 @@
         <v>31</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
@@ -1349,7 +1337,7 @@
       <c r="L6" s="18"/>
       <c r="M6" s="18"/>
       <c r="O6" s="23" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1360,13 +1348,13 @@
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E7" s="14" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -1404,7 +1392,7 @@
       <c r="E9" s="17"/>
       <c r="H9" s="2"/>
       <c r="I9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -1420,7 +1408,7 @@
       <c r="E10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -1437,10 +1425,10 @@
         <v>31</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -1451,7 +1439,7 @@
         <v>16</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E12" s="17"/>
       <c r="I12" s="2"/>
@@ -1470,7 +1458,7 @@
         <v>31</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -1505,7 +1493,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="32"/>
       <c r="G15" s="2" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I15" s="2"/>
     </row>
@@ -1522,7 +1510,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="33"/>
       <c r="G16" s="2" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="I16" s="2"/>
     </row>
@@ -1539,7 +1527,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="34"/>
       <c r="G17" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I17" s="2"/>
     </row>
@@ -1551,12 +1539,12 @@
         <v>30</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="16"/>
       <c r="I18" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.3">
@@ -1623,7 +1611,7 @@
         <v>33</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>36</v>
@@ -1641,31 +1629,31 @@
         <v>39</v>
       </c>
       <c r="J21" s="35" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="K21" s="19" t="s">
         <v>41</v>
       </c>
       <c r="L21" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="M21" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="N21" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="O21" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="P21" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="M21" s="31" t="s">
+      <c r="Q21" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="N21" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="O21" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="P21" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q21" s="31" t="s">
-        <v>63</v>
-      </c>
       <c r="R21" s="11" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.3">
@@ -1673,7 +1661,7 @@
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.3">
@@ -1683,12 +1671,12 @@
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1699,10 +1687,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9EFB2D95-35AE-4AF2-9ECB-D8B602C442C0}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView zoomScale="94" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1710,29 +1698,6 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G28" t="s">
-        <v>44</v>
-      </c>
-      <c r="H28" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="29" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G29" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="30" spans="7:8" x14ac:dyDescent="0.3">
-      <c r="G30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G33" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1767,7 +1732,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="15"/>
@@ -1791,7 +1756,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C3" s="17"/>
       <c r="D3" s="2"/>
@@ -1804,7 +1769,7 @@
         <v>11</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -1827,14 +1792,14 @@
         <v>16</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C6" s="17"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B7" s="19">
         <v>1</v>
@@ -1850,7 +1815,7 @@
         <v>15</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -1863,7 +1828,7 @@
         <v>12</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -1876,7 +1841,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C10" s="2"/>
       <c r="E10" s="2"/>
@@ -1886,7 +1851,7 @@
         <v>40</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C11" s="17"/>
       <c r="D11" s="16"/>
@@ -1928,10 +1893,10 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="11">
         <v>1</v>
@@ -1940,7 +1905,7 @@
         <v>15</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>29</v>
@@ -1949,16 +1914,16 @@
         <v>43</v>
       </c>
       <c r="H14" s="26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I14" s="11"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C15" s="11">
         <f>1/100</f>
@@ -1968,7 +1933,7 @@
         <v>27</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>29</v>
@@ -1977,7 +1942,7 @@
         <v>43</v>
       </c>
       <c r="H15" s="26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I15" s="11"/>
     </row>
@@ -2010,7 +1975,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="2"/>
@@ -2023,7 +1988,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2046,7 +2011,7 @@
         <v>16</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" s="17"/>
       <c r="E4" s="2"/>
@@ -2082,7 +2047,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C7" s="2"/>
       <c r="E7" s="2"/>
@@ -2102,7 +2067,7 @@
         <v>40</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C9" s="17"/>
       <c r="D9" s="16"/>
@@ -2144,10 +2109,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C12" s="11">
         <v>1</v>
@@ -2156,7 +2121,7 @@
         <v>15</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>29</v>
@@ -2165,16 +2130,16 @@
         <v>43</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C13" s="11">
         <v>1</v>
@@ -2183,7 +2148,7 @@
         <v>15</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>29</v>
@@ -2192,7 +2157,7 @@
         <v>43</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I13" s="11"/>
     </row>
@@ -2201,7 +2166,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="2"/>
@@ -2214,7 +2179,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -2237,14 +2202,14 @@
         <v>16</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C18" s="17"/>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B19" s="19">
         <v>1</v>
@@ -2271,7 +2236,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -2333,10 +2298,10 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C26" s="11">
         <v>200</v>
@@ -2345,7 +2310,7 @@
         <v>27</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>29</v>
@@ -2354,16 +2319,16 @@
         <v>43</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I26" s="11"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C27" s="11">
         <v>42</v>
@@ -2372,7 +2337,7 @@
         <v>27</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>29</v>
@@ -2381,25 +2346,25 @@
         <v>43</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I27" s="11"/>
     </row>
     <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="28" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C28" s="11">
         <v>100</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F28" s="11" t="s">
         <v>29</v>
@@ -2408,7 +2373,7 @@
         <v>43</v>
       </c>
       <c r="H28" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I28" s="11"/>
     </row>
@@ -2417,7 +2382,7 @@
         <v>10</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C30" s="17"/>
       <c r="D30" s="2"/>
@@ -2430,7 +2395,7 @@
         <v>11</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -2453,14 +2418,14 @@
         <v>16</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C33" s="17"/>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B34" s="19">
         <v>1</v>
@@ -2488,7 +2453,7 @@
         <v>12</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -2501,7 +2466,7 @@
         <v>26</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -2552,10 +2517,10 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C41" s="11">
         <v>100</v>
@@ -2564,7 +2529,7 @@
         <v>27</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F41" s="11" t="s">
         <v>29</v>
@@ -2573,16 +2538,16 @@
         <v>43</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I41" s="11"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C42" s="11">
         <v>100</v>
@@ -2591,7 +2556,7 @@
         <v>27</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F42" s="11" t="s">
         <v>29</v>
@@ -2600,25 +2565,25 @@
         <v>43</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I42" s="11"/>
     </row>
     <row r="43" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" s="28" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C43" s="11">
         <v>60</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E43" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F43" s="11" t="s">
         <v>29</v>
@@ -2627,7 +2592,7 @@
         <v>43</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I43" s="11"/>
     </row>
@@ -2636,7 +2601,7 @@
         <v>10</v>
       </c>
       <c r="B45" s="19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C45" s="17"/>
       <c r="D45" s="2"/>
@@ -2649,7 +2614,7 @@
         <v>11</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
@@ -2672,14 +2637,14 @@
         <v>16</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C48" s="17"/>
       <c r="E48" s="2"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B49" s="19">
         <v>1</v>
@@ -2707,7 +2672,7 @@
         <v>12</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C51" s="2"/>
       <c r="E51" s="2"/>
@@ -2768,7 +2733,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="28" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B56" s="11" t="s">
         <v>43</v>
@@ -2780,22 +2745,22 @@
         <v>27</v>
       </c>
       <c r="E56" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>42</v>
       </c>
       <c r="G56" s="11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I56" s="11"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="28" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B57" s="11" t="s">
         <v>43</v>
@@ -2807,22 +2772,22 @@
         <v>27</v>
       </c>
       <c r="E57" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F57" s="11" t="s">
         <v>42</v>
       </c>
       <c r="G57" s="11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I57" s="11"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B58" s="11" t="s">
         <v>43</v>
@@ -2831,19 +2796,19 @@
         <v>0.5</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E58" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F58" s="11" t="s">
         <v>42</v>
       </c>
       <c r="G58" s="11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I58" s="11"/>
     </row>
@@ -2876,7 +2841,7 @@
         <v>10</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="2"/>
@@ -2889,7 +2854,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -2912,14 +2877,14 @@
         <v>16</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C4" s="17"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B5" s="19">
         <v>1</v>
@@ -2944,7 +2909,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -2957,7 +2922,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -3008,35 +2973,35 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C12" s="11">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I12" s="11"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C13" s="11">
         <v>1</v>
@@ -3045,14 +3010,14 @@
         <v>15</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="11"/>
       <c r="H13" s="11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I13" s="11"/>
     </row>
@@ -3061,7 +3026,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C15" s="17"/>
       <c r="D15" s="2"/>
@@ -3074,7 +3039,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -3097,17 +3062,17 @@
         <v>16</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C18" s="17"/>
       <c r="D18" s="2" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B19" s="19">
         <v>1</v>
@@ -3126,7 +3091,7 @@
         <v>15</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2">
@@ -3144,7 +3109,7 @@
         <v>12</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -3155,7 +3120,7 @@
         <v>26</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -3165,7 +3130,7 @@
         <v>40</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C23" s="17"/>
       <c r="D23" s="16"/>
@@ -3207,10 +3172,10 @@
     </row>
     <row r="26" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="30" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C26" s="30">
         <f>(10000/60)/2129.16</f>
@@ -3220,25 +3185,25 @@
         <v>15</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F26" s="30" t="s">
         <v>29</v>
       </c>
       <c r="G26" s="30"/>
       <c r="H26" s="30" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I26" s="28" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="30" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C27" s="30">
         <v>33333.33</v>
@@ -3247,25 +3212,25 @@
         <v>27</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F27" s="30" t="s">
         <v>29</v>
       </c>
       <c r="G27" s="30"/>
       <c r="H27" s="30" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I27" s="28" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="C28" s="30">
         <v>1000</v>
@@ -3274,25 +3239,25 @@
         <v>27</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="F28" s="30" t="s">
         <v>29</v>
       </c>
       <c r="G28" s="30"/>
       <c r="H28" s="30" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I28" s="28" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="28" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B29" s="30" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C29" s="30">
         <f>-(C27*0.999)</f>
@@ -3302,17 +3267,17 @@
         <v>27</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F29" s="30" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G29" s="30"/>
       <c r="H29" s="30" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I29" s="30" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -3320,7 +3285,7 @@
         <v>10</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C31" s="17"/>
       <c r="D31" s="2"/>
@@ -3333,7 +3298,7 @@
         <v>11</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -3356,14 +3321,14 @@
         <v>16</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C34" s="17"/>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="19" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B35" s="19">
         <v>1</v>
@@ -3390,7 +3355,7 @@
         <v>12</v>
       </c>
       <c r="B37" s="19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -3403,7 +3368,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -3414,7 +3379,7 @@
         <v>40</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C39" s="17"/>
       <c r="D39" s="16"/>
@@ -3456,7 +3421,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="28" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B42" s="11" t="s">
         <v>43</v>
@@ -3465,19 +3430,19 @@
         <v>100</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F42" s="11" t="s">
         <v>42</v>
       </c>
       <c r="G42" s="11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="H42" s="11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I42" s="11"/>
     </row>

</xml_diff>